<commit_message>
test(data-sheet): modify file to have only one line of values
</commit_message>
<xml_diff>
--- a/src/test/resources/datasheet/ExcelDataSheet.xlsx
+++ b/src/test/resources/datasheet/ExcelDataSheet.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t xml:space="preserve">first_name</t>
   </si>
@@ -36,12 +36,6 @@
   <si>
     <t xml:space="preserve">Doe</t>
   </si>
-  <si>
-    <t xml:space="preserve">Foo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bar</t>
-  </si>
 </sst>
 </file>
 
@@ -55,6 +49,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -114,8 +109,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -139,43 +138,37 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>32</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>24</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>